<commit_message>
528 commit for student
</commit_message>
<xml_diff>
--- a/doc/张非凡.xlsx
+++ b/doc/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>改正dao层错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.27  18：30-21：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>service层的实体管理器和方法的实现与测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.28  13：44-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -633,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -839,6 +851,19 @@
       </c>
       <c r="C24" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
531 commit for test
</commit_message>
<xml_diff>
--- a/doc/张非凡.xlsx
+++ b/doc/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,7 +222,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2019.5.28  13：44-</t>
+    <t>2019.5.29  18：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成对学生表格的读取并存入数据库操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.28  13：44-17：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成student实体的构建并学习poi的基本操作</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -863,7 +875,18 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>